<commit_message>
Amélioration des pages en termes d'informations
</commit_message>
<xml_diff>
--- a/Excel/Activite.xlsx
+++ b/Excel/Activite.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="98">
   <si>
     <t>Sport</t>
   </si>
@@ -505,12 +505,621 @@
 Pratique en compétition Filles – GAF (Compétition - Gym Artistique Féminine), Pratique en compétition Garçons – GAM (Compétition - Gym Artistique Masculine) : 325 €
 Formation – GAF Pré Fed B – GAF (Compétition - Gym Artistique Féminine) : 270 €</t>
   </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Responsable de section :</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Nina Moreau                                        </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Mail : </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">vuc.kayak.canoe@gmail.com                                               </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Tél. : </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">06 79 68 17 48
+</t>
+    </r>
+  </si>
+  <si>
+    <t>Materiel</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Responsable de section : </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Patrick CHARBONNEL 
+(Les cartes professionnelles des encadrants sportifs sont disponibles sur : https://recherche-educateur.sports.gouv.fr/accueil)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Responsable de section : </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Mickaël ETHUIN
+(Les cartes professionnelles des encadrants sportifs sont disponibles sur : https://recherche-educateur.sports.gouv.fr/accueil)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Responsable de section : </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Thierry VIGNAUX 
+(Les cartes professionnelles des encadrants sportifs sont disponibles sur : https://recherche-educateur.sports.gouv.fr/accueil)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Responsable de section : </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Karim MARION 
+(Les cartes professionnelles des encadrants sportifs sont disponibles sur : https://recherche-educateur.sports.gouv.fr/accueil)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Responsable de section : </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Martial GRISLIN 
+(Les cartes professionnelles des encadrants sportifs sont disponibles sur : https://recherche-educateur.sports.gouv.fr/accueil)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Responsable de section :</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Pascal REP
+(Les cartes professionnelles des encadrants sportifs sont disponibles sur : https://recherche-educateur.sports.gouv.fr/accueil)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Responsable de section :</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Emmanuelle BOUGUERRA  
+(Les cartes professionnelles des encadrants sportifs sont disponibles sur : https://recherche-educateur.sports.gouv.fr/accueil)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Tél. :</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 06 50 52 54 74  
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Mail : </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">gymnastique.vuc@gmail.com
+</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Responsable de section :</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Didier MORAUX 
+(Les cartes professionnelles des encadrants sportifs sont disponibles sur : https://recherche-educateur.sports.gouv.fr/accueil)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Responsable de section :</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Nicolas DEVEMY  
+(Les cartes professionnelles des encadrants sportifs sont disponibles sur : https://recherche-educateur.sports.gouv.fr/accueil)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Mail : </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">C59014@ffaviron.fr  
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Mail 2 : </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">aviron@vuc-omnisports.fr  
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Tél. :</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 06 60 80 97 56
+</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Responsable de section :</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Nina Moreau  
+(Les cartes professionnelles des encadrants sportifs sont disponibles sur : https://recherche-educateur.sports.gouv.fr/accueil)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Mail : </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">vuc.kayak.canoe@gmail.com                                          
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Tél. : </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">06 79 68 17 48
+</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Responsable de section : </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Eric CATTAN  
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Mail : </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">escalade@vuc-omnisports.fr
+</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Responsable de section :</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Emmanuelle BOUGUERRA  
+(Les cartes professionnelles des encadrants sportifs sont disponibles sur : https://recherche-educateur.sports.gouv.fr/accueil)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Tél. :</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 06 50 52 54 74  
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Mail : </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">gymnastique.vuc@gmail.com
+</t>
+    </r>
+  </si>
+  <si>
+    <t>Condition d'accès :
+Présenter un certificat médical de non contre indication à la pratique de l'aviron</t>
+  </si>
+  <si>
+    <t>Condition d'accès :
+Présenter un certificat médical de non contre indication à la pratique du badminton (questionnaire médical pour les mineurs)</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Document obligatoire : </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Présenter un certificat médical
+Savoir nager
+</t>
+    </r>
+  </si>
+  <si>
+    <t>Document obligatoire : 
+Présenter un certificat médical</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Né(e)s en 2022/2023 Mercredi 10h00–11h00 / Samedi 9h00–10h00 , Né(e)s en 2021 Mercredi 11h00–12h00 / Samedi 10h00–11h00, Né(e)s en 2020/2021 Mardi 17h00–18h00 / Samedi 9h00–10h00, Né(e)s en 2020 Samedi 11h00–12h00, Tous (2020 à 2023) Vendredi 17h00–18h00 : 200€ 
+</t>
+  </si>
+  <si>
+    <t>Responsable de section : Otman Bennani</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="9">
+  <fonts count="11">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -568,6 +1177,23 @@
       <color rgb="FF559189"/>
       <name val="&quot;Roboto Mono&quot;"/>
     </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -583,7 +1209,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -591,47 +1217,32 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -644,6 +1255,39 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -864,14 +1508,14 @@
   </sheetPr>
   <dimension ref="A1:R25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="54" zoomScaleNormal="54" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="54" zoomScaleNormal="54" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="35.453125" customWidth="1"/>
-    <col min="2" max="2" width="70" customWidth="1"/>
+    <col min="2" max="2" width="98" customWidth="1"/>
     <col min="3" max="4" width="57" customWidth="1"/>
     <col min="5" max="5" width="72.36328125" customWidth="1"/>
     <col min="6" max="6" width="98.1796875" customWidth="1"/>
@@ -880,575 +1524,625 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="33" customHeight="1">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="D1" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="E1" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="3"/>
-      <c r="N1" s="3"/>
-      <c r="O1" s="3"/>
-      <c r="P1" s="3"/>
-      <c r="Q1" s="3"/>
-      <c r="R1" s="3"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
+      <c r="P1" s="2"/>
+      <c r="Q1" s="2"/>
+      <c r="R1" s="2"/>
     </row>
     <row r="2" spans="1:18" ht="409.6" customHeight="1">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="1" t="s">
+      <c r="C2" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="E2" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G2" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="H2" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
-      <c r="L2" s="2"/>
-      <c r="M2" s="3"/>
-      <c r="N2" s="3"/>
-      <c r="O2" s="3"/>
-      <c r="P2" s="3"/>
-      <c r="Q2" s="3"/>
-      <c r="R2" s="3"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+      <c r="O2" s="2"/>
+      <c r="P2" s="2"/>
+      <c r="Q2" s="2"/>
+      <c r="R2" s="2"/>
     </row>
     <row r="3" spans="1:18" ht="345.5" customHeight="1">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="1" t="s">
+      <c r="C3" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="E3" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F3" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="G3" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="H3" s="5" t="s">
+      <c r="H3" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
-      <c r="L3" s="2"/>
-      <c r="M3" s="3"/>
-      <c r="N3" s="3"/>
-      <c r="O3" s="3"/>
-      <c r="P3" s="3"/>
-      <c r="Q3" s="3"/>
-      <c r="R3" s="3"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+      <c r="O3" s="2"/>
+      <c r="P3" s="2"/>
+      <c r="Q3" s="2"/>
+      <c r="R3" s="2"/>
     </row>
     <row r="4" spans="1:18" ht="133.5" customHeight="1">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="1" t="s">
+      <c r="C4" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="E4" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="F4" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="G4" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="H4" s="5" t="s">
+      <c r="H4" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
-      <c r="L4" s="2"/>
-      <c r="M4" s="3"/>
-      <c r="N4" s="3"/>
-      <c r="O4" s="3"/>
-      <c r="P4" s="3"/>
-      <c r="Q4" s="3"/>
-      <c r="R4" s="3"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
+      <c r="O4" s="2"/>
+      <c r="P4" s="2"/>
+      <c r="Q4" s="2"/>
+      <c r="R4" s="2"/>
     </row>
     <row r="5" spans="1:18" ht="387.5">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E5" s="1" t="s">
+      <c r="C5" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="E5" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="F5" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="G5" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="H5" s="5" t="s">
+      <c r="H5" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
-      <c r="K5" s="2"/>
-      <c r="L5" s="2"/>
-      <c r="M5" s="3"/>
-      <c r="N5" s="3"/>
-      <c r="O5" s="3"/>
-      <c r="P5" s="3"/>
-      <c r="Q5" s="3"/>
-      <c r="R5" s="3"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
+      <c r="O5" s="2"/>
+      <c r="P5" s="2"/>
+      <c r="Q5" s="2"/>
+      <c r="R5" s="2"/>
     </row>
     <row r="6" spans="1:18" ht="341">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="1" t="s">
+      <c r="C6" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>94</v>
+      </c>
+      <c r="E6" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="F6" s="8" t="s">
+      <c r="F6" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="G6" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="H6" s="5" t="s">
+      <c r="H6" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
-      <c r="K6" s="2"/>
-      <c r="L6" s="2"/>
-      <c r="M6" s="3"/>
-      <c r="N6" s="3"/>
-      <c r="O6" s="3"/>
-      <c r="P6" s="3"/>
-      <c r="Q6" s="3"/>
-      <c r="R6" s="3"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
+      <c r="O6" s="2"/>
+      <c r="P6" s="2"/>
+      <c r="Q6" s="2"/>
+      <c r="R6" s="2"/>
     </row>
     <row r="7" spans="1:18" ht="192" customHeight="1">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="1" t="s">
+      <c r="C7" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="E7" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="F7" s="8" t="s">
+      <c r="F7" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="G7" s="1" t="s">
+      <c r="G7" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="H7" s="5" t="s">
+      <c r="H7" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="I7" s="2"/>
-      <c r="J7" s="2"/>
-      <c r="K7" s="2"/>
-      <c r="L7" s="2"/>
-      <c r="M7" s="3"/>
-      <c r="N7" s="3"/>
-      <c r="O7" s="3"/>
-      <c r="P7" s="3"/>
-      <c r="Q7" s="3"/>
-      <c r="R7" s="3"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
+      <c r="M7" s="2"/>
+      <c r="N7" s="2"/>
+      <c r="O7" s="2"/>
+      <c r="P7" s="2"/>
+      <c r="Q7" s="2"/>
+      <c r="R7" s="2"/>
     </row>
     <row r="8" spans="1:18" ht="144" customHeight="1">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="1" t="s">
+      <c r="C8" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="D8" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="E8" s="8"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="H8" s="5" t="s">
+      <c r="H8" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="I8" s="2"/>
-      <c r="J8" s="2"/>
-      <c r="K8" s="2"/>
-      <c r="L8" s="2"/>
-      <c r="M8" s="3"/>
-      <c r="N8" s="3"/>
-      <c r="O8" s="3"/>
-      <c r="P8" s="3"/>
-      <c r="Q8" s="3"/>
-      <c r="R8" s="3"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+      <c r="L8" s="1"/>
+      <c r="M8" s="2"/>
+      <c r="N8" s="2"/>
+      <c r="O8" s="2"/>
+      <c r="P8" s="2"/>
+      <c r="Q8" s="2"/>
+      <c r="R8" s="2"/>
     </row>
     <row r="9" spans="1:18" ht="135" customHeight="1">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="1" t="s">
+      <c r="C9" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="D9" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="E9" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="F9" s="8" t="s">
+      <c r="F9" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="G9" s="1" t="s">
+      <c r="G9" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="H9" s="5" t="s">
+      <c r="H9" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="I9" s="2"/>
-      <c r="J9" s="2"/>
-      <c r="K9" s="2"/>
-      <c r="L9" s="2"/>
-      <c r="M9" s="3"/>
-      <c r="N9" s="3"/>
-      <c r="O9" s="3"/>
-      <c r="P9" s="3"/>
-      <c r="Q9" s="3"/>
-      <c r="R9" s="3"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+      <c r="L9" s="1"/>
+      <c r="M9" s="2"/>
+      <c r="N9" s="2"/>
+      <c r="O9" s="2"/>
+      <c r="P9" s="2"/>
+      <c r="Q9" s="2"/>
+      <c r="R9" s="2"/>
     </row>
     <row r="10" spans="1:18" ht="172.5" customHeight="1">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="1" t="s">
+      <c r="C10" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="D10" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="E10" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="F10" s="8" t="s">
+      <c r="F10" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="G10" s="1" t="s">
+      <c r="G10" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="H10" s="5" t="s">
+      <c r="H10" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="I10" s="2"/>
-      <c r="J10" s="2"/>
-      <c r="K10" s="2"/>
-      <c r="L10" s="2"/>
-      <c r="M10" s="3"/>
-      <c r="N10" s="3"/>
-      <c r="O10" s="3"/>
-      <c r="P10" s="3"/>
-      <c r="Q10" s="3"/>
-      <c r="R10" s="3"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
+      <c r="L10" s="1"/>
+      <c r="M10" s="2"/>
+      <c r="N10" s="2"/>
+      <c r="O10" s="2"/>
+      <c r="P10" s="2"/>
+      <c r="Q10" s="2"/>
+      <c r="R10" s="2"/>
     </row>
     <row r="11" spans="1:18" ht="230.5" customHeight="1">
-      <c r="A11" s="1" t="s">
+      <c r="A11" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="1" t="s">
+      <c r="C11" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="D11" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="E11" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="F11" s="8" t="s">
+      <c r="F11" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="G11" s="1" t="s">
+      <c r="G11" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="H11" s="5" t="s">
+      <c r="H11" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="I11" s="2"/>
-      <c r="J11" s="2"/>
-      <c r="K11" s="2"/>
-      <c r="L11" s="2"/>
-      <c r="M11" s="3"/>
-      <c r="N11" s="3"/>
-      <c r="O11" s="3"/>
-      <c r="P11" s="3"/>
-      <c r="Q11" s="3"/>
-      <c r="R11" s="3"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1"/>
+      <c r="L11" s="1"/>
+      <c r="M11" s="2"/>
+      <c r="N11" s="2"/>
+      <c r="O11" s="2"/>
+      <c r="P11" s="2"/>
+      <c r="Q11" s="2"/>
+      <c r="R11" s="2"/>
     </row>
     <row r="12" spans="1:18" ht="356.5">
-      <c r="A12" s="1" t="s">
+      <c r="A12" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="1" t="s">
+      <c r="C12" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="F12" s="8" t="s">
+      <c r="F12" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="G12" s="10" t="s">
+      <c r="G12" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="H12" s="11" t="s">
+      <c r="H12" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="I12" s="2"/>
-      <c r="J12" s="2"/>
-      <c r="K12" s="2"/>
-      <c r="L12" s="2"/>
-      <c r="M12" s="3"/>
-      <c r="N12" s="3"/>
-      <c r="O12" s="3"/>
-      <c r="P12" s="3"/>
-      <c r="Q12" s="3"/>
-      <c r="R12" s="3"/>
-    </row>
-    <row r="13" spans="1:18" ht="217">
-      <c r="A13" s="1" t="s">
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
+      <c r="L12" s="1"/>
+      <c r="M12" s="2"/>
+      <c r="N12" s="2"/>
+      <c r="O12" s="2"/>
+      <c r="P12" s="2"/>
+      <c r="Q12" s="2"/>
+      <c r="R12" s="2"/>
+    </row>
+    <row r="13" spans="1:18" ht="241" customHeight="1">
+      <c r="A13" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="1" t="s">
+      <c r="C13" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="D13" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="E13" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="F13" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="G13" s="12" t="s">
+      <c r="F13" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="G13" s="18" t="s">
         <v>66</v>
       </c>
-      <c r="H13" s="11" t="s">
+      <c r="H13" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="I13" s="13"/>
-      <c r="J13" s="13"/>
-      <c r="K13" s="13"/>
-      <c r="L13" s="13"/>
-      <c r="M13" s="14"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="3"/>
+      <c r="K13" s="3"/>
+      <c r="L13" s="3"/>
+      <c r="M13" s="4"/>
     </row>
     <row r="14" spans="1:18" ht="409.6" customHeight="1">
-      <c r="A14" s="1" t="s">
+      <c r="A14" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="1" t="s">
+      <c r="C14" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="D14" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="E14" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="F14" s="8" t="s">
+      <c r="F14" s="15" t="s">
         <v>77</v>
       </c>
-      <c r="G14" s="12" t="s">
+      <c r="G14" s="18" t="s">
         <v>70</v>
       </c>
-      <c r="H14" s="5" t="s">
+      <c r="H14" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="I14" s="13"/>
-      <c r="J14" s="13"/>
-      <c r="K14" s="13"/>
-      <c r="L14" s="13"/>
-      <c r="M14" s="14"/>
+      <c r="I14" s="3"/>
+      <c r="J14" s="3"/>
+      <c r="K14" s="3"/>
+      <c r="L14" s="3"/>
+      <c r="M14" s="4"/>
     </row>
     <row r="15" spans="1:18" ht="409.5" customHeight="1">
-      <c r="A15" s="1" t="s">
+      <c r="A15" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="1" t="s">
+      <c r="C15" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="D15" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="E15" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="F15" s="8" t="s">
+      <c r="F15" s="15" t="s">
         <v>74</v>
       </c>
-      <c r="G15" s="1" t="s">
+      <c r="G15" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="H15" s="5" t="s">
+      <c r="H15" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="I15" s="13"/>
-      <c r="J15" s="13"/>
-      <c r="K15" s="13"/>
-      <c r="L15" s="13"/>
-      <c r="M15" s="14"/>
+      <c r="I15" s="3"/>
+      <c r="J15" s="3"/>
+      <c r="K15" s="3"/>
+      <c r="L15" s="3"/>
+      <c r="M15" s="4"/>
     </row>
     <row r="16" spans="1:18" ht="15.5">
-      <c r="A16" s="13"/>
-      <c r="B16" s="13"/>
-      <c r="C16" s="13"/>
-      <c r="D16" s="13"/>
-      <c r="E16" s="13"/>
-      <c r="F16" s="15"/>
-      <c r="G16" s="13"/>
-      <c r="H16" s="13"/>
-      <c r="I16" s="13"/>
-      <c r="J16" s="13"/>
-      <c r="K16" s="13"/>
-      <c r="L16" s="13"/>
-      <c r="M16" s="14"/>
+      <c r="A16" s="3"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="3"/>
+      <c r="J16" s="3"/>
+      <c r="K16" s="3"/>
+      <c r="L16" s="3"/>
+      <c r="M16" s="4"/>
     </row>
     <row r="17" spans="1:13" ht="15.5">
-      <c r="A17" s="13"/>
-      <c r="B17" s="13"/>
-      <c r="C17" s="13"/>
-      <c r="D17" s="13"/>
-      <c r="E17" s="13"/>
-      <c r="F17" s="15"/>
-      <c r="G17" s="13"/>
-      <c r="H17" s="13"/>
-      <c r="I17" s="13"/>
-      <c r="J17" s="13"/>
-      <c r="K17" s="13"/>
-      <c r="L17" s="13"/>
-      <c r="M17" s="14"/>
+      <c r="A17" s="3"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="3"/>
+      <c r="J17" s="3"/>
+      <c r="K17" s="3"/>
+      <c r="L17" s="3"/>
+      <c r="M17" s="4"/>
     </row>
     <row r="18" spans="1:13" ht="15.5">
-      <c r="A18" s="13"/>
-      <c r="B18" s="13"/>
-      <c r="C18" s="13"/>
-      <c r="D18" s="13"/>
-      <c r="E18" s="13"/>
-      <c r="F18" s="15"/>
-      <c r="G18" s="13"/>
-      <c r="H18" s="13"/>
-      <c r="I18" s="13"/>
-      <c r="J18" s="13"/>
-      <c r="K18" s="13"/>
-      <c r="L18" s="13"/>
-      <c r="M18" s="14"/>
+      <c r="A18" s="3"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
+      <c r="I18" s="3"/>
+      <c r="J18" s="3"/>
+      <c r="K18" s="3"/>
+      <c r="L18" s="3"/>
+      <c r="M18" s="4"/>
     </row>
     <row r="19" spans="1:13" ht="15.5">
-      <c r="A19" s="13"/>
-      <c r="B19" s="13"/>
-      <c r="C19" s="13"/>
-      <c r="D19" s="13"/>
-      <c r="E19" s="13"/>
-      <c r="F19" s="15"/>
-      <c r="G19" s="13"/>
-      <c r="H19" s="13"/>
-      <c r="I19" s="13"/>
-      <c r="J19" s="13"/>
-      <c r="K19" s="13"/>
-      <c r="L19" s="13"/>
-      <c r="M19" s="14"/>
+      <c r="A19" s="3"/>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
+      <c r="I19" s="3"/>
+      <c r="J19" s="3"/>
+      <c r="K19" s="3"/>
+      <c r="L19" s="3"/>
+      <c r="M19" s="4"/>
     </row>
     <row r="20" spans="1:13" ht="15.5">
-      <c r="A20" s="13"/>
-      <c r="B20" s="13"/>
-      <c r="C20" s="13"/>
-      <c r="D20" s="13"/>
-      <c r="E20" s="16"/>
-      <c r="F20" s="15"/>
-      <c r="G20" s="13"/>
-      <c r="H20" s="13"/>
-      <c r="I20" s="13"/>
-      <c r="J20" s="13"/>
-      <c r="K20" s="13"/>
-      <c r="L20" s="13"/>
-      <c r="M20" s="14"/>
+      <c r="A20" s="3"/>
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="5"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
+      <c r="I20" s="3"/>
+      <c r="J20" s="3"/>
+      <c r="K20" s="3"/>
+      <c r="L20" s="3"/>
+      <c r="M20" s="4"/>
     </row>
     <row r="21" spans="1:13" ht="15.5">
-      <c r="A21" s="13"/>
-      <c r="B21" s="13"/>
-      <c r="C21" s="13"/>
-      <c r="D21" s="13"/>
-      <c r="E21" s="13"/>
-      <c r="F21" s="15"/>
-      <c r="G21" s="13"/>
-      <c r="H21" s="13"/>
-      <c r="I21" s="13"/>
-      <c r="J21" s="13"/>
-      <c r="K21" s="13"/>
-      <c r="L21" s="13"/>
-      <c r="M21" s="14"/>
+      <c r="A21" s="3"/>
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="3"/>
+      <c r="H21" s="3"/>
+      <c r="I21" s="3"/>
+      <c r="J21" s="3"/>
+      <c r="K21" s="3"/>
+      <c r="L21" s="3"/>
+      <c r="M21" s="4"/>
     </row>
     <row r="22" spans="1:13" ht="14">
-      <c r="F22" s="17"/>
+      <c r="F22" s="7"/>
     </row>
     <row r="23" spans="1:13" ht="14">
-      <c r="F23" s="17"/>
+      <c r="F23" s="7"/>
     </row>
     <row r="24" spans="1:13" ht="14">
-      <c r="F24" s="17"/>
+      <c r="F24" s="7"/>
     </row>
     <row r="25" spans="1:13" ht="14">
-      <c r="F25" s="17"/>
+      <c r="F25" s="7"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1468,5 +2162,6 @@
     <hyperlink ref="H15" r:id="rId14"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId15"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Changement de acceuiL;tml à index.html pour la mise en ligne
</commit_message>
<xml_diff>
--- a/Excel/Activite.xlsx
+++ b/Excel/Activite.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="94">
   <si>
     <t>Sport</t>
   </si>
@@ -28,9 +28,6 @@
   </si>
   <si>
     <t>Contact</t>
-  </si>
-  <si>
-    <t>Matériel</t>
   </si>
   <si>
     <t>Horaires</t>
@@ -165,12 +162,6 @@
                 Un ballet sur l’eau… à fond les rames !</t>
   </si>
   <si>
-    <t>ffbb</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bdb  </t>
-  </si>
-  <si>
     <t>Mardi
 Compétiteurs
 18 h 00 – 20 h 00
@@ -423,14 +414,6 @@
 → Samedi de 11 h 00 à 12 h 00</t>
   </si>
   <si>
-    <t xml:space="preserve">Né(e)s en 2022/2023 : 200 € | Mercredi 10h00–11h00 / Samedi 9h00–10h00  
-Né(e)s en 2021       : 200 € | Mercredi 11h00–12h00 / Samedi 10h00–11h00  
-Né(e)s en 2020/2021  : 200 € | Mardi 17h00–18h00 / Samedi 9h00–10h00  
-Né(e)s en 2020       : 200 € | Samedi 11h00–12h00  
-Tous (2020 à 2023)   : 200 € | Vendredi 17h00–18h00  
-</t>
-  </si>
-  <si>
     <t>Salle Jean Chanat
 Chemin des Bourgeois
 VALENCIENNES</t>
@@ -506,75 +489,6 @@
 Formation – GAF Pré Fed B – GAF (Compétition - Gym Artistique Féminine) : 270 €</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Responsable de section :</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Nina Moreau                                        </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Mail : </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">vuc.kayak.canoe@gmail.com                                               </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Tél. : </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">06 79 68 17 48
-</t>
-    </r>
-  </si>
-  <si>
     <t>Materiel</t>
   </si>
   <si>
@@ -1068,51 +982,34 @@
     </r>
   </si>
   <si>
+    <t xml:space="preserve">Né(e)s en 2022/2023 Mercredi 10h00–11h00 / Samedi 9h00–10h00 , Né(e)s en 2021 Mercredi 11h00–12h00 / Samedi 10h00–11h00, Né(e)s en 2020/2021 Mardi 17h00–18h00 / Samedi 9h00–10h00, Né(e)s en 2020 Samedi 11h00–12h00, Tous (2020 à 2023) Vendredi 17h00–18h00 : 200€ 
+</t>
+  </si>
+  <si>
+    <t>Responsable de section : Otman Bennani</t>
+  </si>
+  <si>
     <t>Condition d'accès :
-Présenter un certificat médical de non contre indication à la pratique de l'aviron</t>
+Questionnaire médical à remplir lors de l'inscription en ligne de non contre indication à la pratique du badminton (questionnaire médical pour les mineurs)</t>
+  </si>
+  <si>
+    <t>Document obligatoire : 
+Questionnaire médical à remplir lors de l'inscription en ligne</t>
   </si>
   <si>
     <t>Condition d'accès :
-Présenter un certificat médical de non contre indication à la pratique du badminton (questionnaire médical pour les mineurs)</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Document obligatoire : </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Présenter un certificat médical
+Questionnaire médical à remplir lors de l'inscription en ligne de non contre indication à la pratique de l'aviron</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Document obligatoire : 
+Questionnaire médical à remplir lors de l'inscription en ligne
 Savoir nager
 </t>
-    </r>
-  </si>
-  <si>
-    <t>Document obligatoire : 
-Présenter un certificat médical</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Né(e)s en 2022/2023 Mercredi 10h00–11h00 / Samedi 9h00–10h00 , Né(e)s en 2021 Mercredi 11h00–12h00 / Samedi 10h00–11h00, Né(e)s en 2020/2021 Mardi 17h00–18h00 / Samedi 9h00–10h00, Né(e)s en 2020 Samedi 11h00–12h00, Tous (2020 à 2023) Vendredi 17h00–18h00 : 200€ 
-</t>
-  </si>
-  <si>
-    <t>Responsable de section : Otman Bennani</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Document obligatoire : 
+Questionnaire médical à remplir lors de l'inscription en ligne </t>
   </si>
 </sst>
 </file>
@@ -1508,8 +1405,8 @@
   </sheetPr>
   <dimension ref="A1:R25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="54" zoomScaleNormal="54" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="54" zoomScaleNormal="54" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1"/>
@@ -1534,19 +1431,19 @@
         <v>2</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="E1" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="G1" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="12" t="s">
+      <c r="H1" s="12" t="s">
         <v>6</v>
-      </c>
-      <c r="H1" s="12" t="s">
-        <v>7</v>
       </c>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
@@ -1561,28 +1458,28 @@
     </row>
     <row r="2" spans="1:18" ht="409.6" customHeight="1">
       <c r="A2" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="C2" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="E2" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="12" t="s">
-        <v>80</v>
-      </c>
-      <c r="D2" s="13" t="s">
-        <v>93</v>
-      </c>
-      <c r="E2" s="8" t="s">
+      <c r="F2" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="G2" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="H2" s="14" t="s">
         <v>12</v>
-      </c>
-      <c r="H2" s="14" t="s">
-        <v>13</v>
       </c>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
@@ -1597,28 +1494,28 @@
     </row>
     <row r="3" spans="1:18" ht="345.5" customHeight="1">
       <c r="A3" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="C3" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="E3" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="12" t="s">
-        <v>87</v>
-      </c>
-      <c r="D3" s="13" t="s">
-        <v>95</v>
-      </c>
-      <c r="E3" s="8" t="s">
+      <c r="F3" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="8" t="s">
+      <c r="G3" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="G3" s="8" t="s">
-        <v>18</v>
-      </c>
       <c r="H3" s="14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
@@ -1633,28 +1530,28 @@
     </row>
     <row r="4" spans="1:18" ht="133.5" customHeight="1">
       <c r="A4" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="C4" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="E4" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="12" t="s">
-        <v>81</v>
-      </c>
-      <c r="D4" s="13" t="s">
-        <v>95</v>
-      </c>
-      <c r="E4" s="8" t="s">
+      <c r="F4" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="F4" s="8" t="s">
+      <c r="G4" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="G4" s="8" t="s">
-        <v>23</v>
-      </c>
       <c r="H4" s="14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
@@ -1669,28 +1566,28 @@
     </row>
     <row r="5" spans="1:18" ht="387.5">
       <c r="A5" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="C5" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="E5" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C5" s="13" t="s">
-        <v>88</v>
-      </c>
-      <c r="D5" s="13" t="s">
-        <v>92</v>
-      </c>
-      <c r="E5" s="8" t="s">
-        <v>28</v>
-      </c>
       <c r="F5" s="8" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="H5" s="14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
@@ -1705,28 +1602,28 @@
     </row>
     <row r="6" spans="1:18" ht="341">
       <c r="A6" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="F6" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="G6" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="C6" s="13" t="s">
-        <v>89</v>
-      </c>
-      <c r="D6" s="13" t="s">
-        <v>94</v>
-      </c>
-      <c r="E6" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="F6" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="G6" s="8" t="s">
-        <v>35</v>
-      </c>
       <c r="H6" s="14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
@@ -1741,28 +1638,28 @@
     </row>
     <row r="7" spans="1:18" ht="192" customHeight="1">
       <c r="A7" s="12" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B7" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="F7" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="G7" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="C7" s="12" t="s">
-        <v>82</v>
-      </c>
-      <c r="D7" s="13" t="s">
-        <v>95</v>
-      </c>
-      <c r="E7" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="F7" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="G7" s="8" t="s">
-        <v>39</v>
-      </c>
       <c r="H7" s="14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
@@ -1777,24 +1674,24 @@
     </row>
     <row r="8" spans="1:18" ht="144" customHeight="1">
       <c r="A8" s="12" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="D8" s="13" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="E8" s="8"/>
       <c r="F8" s="15"/>
       <c r="G8" s="8" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="H8" s="14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
@@ -1809,28 +1706,28 @@
     </row>
     <row r="9" spans="1:18" ht="135" customHeight="1">
       <c r="A9" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="D9" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="F9" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="G9" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="C9" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="D9" s="13" t="s">
-        <v>95</v>
-      </c>
-      <c r="E9" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="F9" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="G9" s="8" t="s">
-        <v>46</v>
-      </c>
       <c r="H9" s="14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
@@ -1845,28 +1742,28 @@
     </row>
     <row r="10" spans="1:18" ht="172.5" customHeight="1">
       <c r="A10" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="D10" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="F10" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="G10" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="C10" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="D10" s="13" t="s">
-        <v>95</v>
-      </c>
-      <c r="E10" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="F10" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="G10" s="8" t="s">
-        <v>51</v>
-      </c>
       <c r="H10" s="14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
@@ -1881,28 +1778,28 @@
     </row>
     <row r="11" spans="1:18" ht="230.5" customHeight="1">
       <c r="A11" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="D11" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="F11" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="G11" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="C11" s="12" t="s">
-        <v>85</v>
-      </c>
-      <c r="D11" s="13" t="s">
-        <v>95</v>
-      </c>
-      <c r="E11" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="F11" s="15" t="s">
-        <v>55</v>
-      </c>
-      <c r="G11" s="8" t="s">
-        <v>56</v>
-      </c>
       <c r="H11" s="14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
@@ -1917,26 +1814,26 @@
     </row>
     <row r="12" spans="1:18" ht="356.5">
       <c r="A12" s="12" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C12" s="13" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="D12" s="8"/>
       <c r="E12" s="8" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="F12" s="15" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="G12" s="16" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="H12" s="17" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
@@ -1951,28 +1848,28 @@
     </row>
     <row r="13" spans="1:18" ht="241" customHeight="1">
       <c r="A13" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="D13" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="F13" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="G13" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="B13" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="C13" s="13" t="s">
-        <v>91</v>
-      </c>
-      <c r="D13" s="13" t="s">
-        <v>95</v>
-      </c>
-      <c r="E13" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="F13" s="15" t="s">
-        <v>96</v>
-      </c>
-      <c r="G13" s="18" t="s">
-        <v>66</v>
-      </c>
       <c r="H13" s="17" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I13" s="3"/>
       <c r="J13" s="3"/>
@@ -1982,28 +1879,28 @@
     </row>
     <row r="14" spans="1:18" ht="409.6" customHeight="1">
       <c r="A14" s="12" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C14" s="13" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="D14" s="13" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="F14" s="15" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="G14" s="18" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="H14" s="14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I14" s="3"/>
       <c r="J14" s="3"/>
@@ -2013,28 +1910,28 @@
     </row>
     <row r="15" spans="1:18" ht="409.5" customHeight="1">
       <c r="A15" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="C15" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="D15" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="F15" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="G15" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="B15" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="C15" s="13" t="s">
-        <v>91</v>
-      </c>
-      <c r="D15" s="13" t="s">
-        <v>95</v>
-      </c>
-      <c r="E15" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="F15" s="15" t="s">
-        <v>74</v>
-      </c>
-      <c r="G15" s="8" t="s">
-        <v>75</v>
-      </c>
       <c r="H15" s="14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I15" s="3"/>
       <c r="J15" s="3"/>

</xml_diff>